<commit_message>
fix: add ticket to db schema
</commit_message>
<xml_diff>
--- a/__fixtures__/simple.xlsx
+++ b/__fixtures__/simple.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B7DDB1-22CD-9A4E-81BD-916D9ECD56BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3155266-58A5-A14C-B433-F7C59CCDC0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
   <si>
     <t>Address</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>test@email.com</t>
+  </si>
+  <si>
+    <t>Y23-ticket</t>
+  </si>
+  <si>
+    <t>2;3</t>
   </si>
 </sst>
 </file>
@@ -672,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG3"/>
+  <dimension ref="A1:BH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AS1" sqref="AS1:AS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -691,12 +697,13 @@
     <col min="37" max="37" width="19.6640625" customWidth="1"/>
     <col min="38" max="38" width="16" customWidth="1"/>
     <col min="39" max="39" width="40" customWidth="1"/>
+    <col min="44" max="44" width="24.83203125" customWidth="1"/>
     <col min="46" max="46" width="27.6640625" customWidth="1"/>
     <col min="47" max="47" width="47" customWidth="1"/>
-    <col min="57" max="57" width="16" customWidth="1"/>
+    <col min="58" max="58" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -845,37 +852,40 @@
         <v>48</v>
       </c>
       <c r="AX1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -943,16 +953,19 @@
         <v>1</v>
       </c>
       <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
-        <v>0</v>
-      </c>
-      <c r="BG2">
+        <v>5</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1052,34 +1065,37 @@
       <c r="AW3">
         <v>1</v>
       </c>
-      <c r="AX3">
+      <c r="AX3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY3">
         <v>1</v>
       </c>
-      <c r="AY3" t="s">
+      <c r="AZ3" t="s">
         <v>62</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BA3" t="s">
         <v>63</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BB3" t="s">
         <v>64</v>
       </c>
-      <c r="BB3">
-        <v>0</v>
-      </c>
       <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3">
         <v>1</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BE3" t="s">
         <v>62</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BF3" t="s">
         <v>65</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BG3" t="s">
         <v>64</v>
       </c>
-      <c r="BG3">
+      <c r="BH3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: ability to record ticket per event (#70)
</commit_message>
<xml_diff>
--- a/__fixtures__/simple.xlsx
+++ b/__fixtures__/simple.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B7DDB1-22CD-9A4E-81BD-916D9ECD56BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3155266-58A5-A14C-B433-F7C59CCDC0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
   <si>
     <t>Address</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>test@email.com</t>
+  </si>
+  <si>
+    <t>Y23-ticket</t>
+  </si>
+  <si>
+    <t>2;3</t>
   </si>
 </sst>
 </file>
@@ -672,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG3"/>
+  <dimension ref="A1:BH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AS1" sqref="AS1:AS1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -691,12 +697,13 @@
     <col min="37" max="37" width="19.6640625" customWidth="1"/>
     <col min="38" max="38" width="16" customWidth="1"/>
     <col min="39" max="39" width="40" customWidth="1"/>
+    <col min="44" max="44" width="24.83203125" customWidth="1"/>
     <col min="46" max="46" width="27.6640625" customWidth="1"/>
     <col min="47" max="47" width="47" customWidth="1"/>
-    <col min="57" max="57" width="16" customWidth="1"/>
+    <col min="58" max="58" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -845,37 +852,40 @@
         <v>48</v>
       </c>
       <c r="AX1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AY1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>57</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -943,16 +953,19 @@
         <v>1</v>
       </c>
       <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
-        <v>0</v>
-      </c>
-      <c r="BG2">
+        <v>5</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+      <c r="BD2">
+        <v>0</v>
+      </c>
+      <c r="BH2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1052,34 +1065,37 @@
       <c r="AW3">
         <v>1</v>
       </c>
-      <c r="AX3">
+      <c r="AX3" t="s">
+        <v>91</v>
+      </c>
+      <c r="AY3">
         <v>1</v>
       </c>
-      <c r="AY3" t="s">
+      <c r="AZ3" t="s">
         <v>62</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BA3" t="s">
         <v>63</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BB3" t="s">
         <v>64</v>
       </c>
-      <c r="BB3">
-        <v>0</v>
-      </c>
       <c r="BC3">
+        <v>0</v>
+      </c>
+      <c r="BD3">
         <v>1</v>
       </c>
-      <c r="BD3" t="s">
+      <c r="BE3" t="s">
         <v>62</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BF3" t="s">
         <v>65</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BG3" t="s">
         <v>64</v>
       </c>
-      <c r="BG3">
+      <c r="BH3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: record ticket sale
</commit_message>
<xml_diff>
--- a/__fixtures__/simple.xlsx
+++ b/__fixtures__/simple.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3155266-58A5-A14C-B433-F7C59CCDC0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92907122-837B-CB4C-A6DD-11192E975B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
   <si>
     <t>Address</t>
   </si>
@@ -290,7 +290,13 @@
     <t>Y23-ticket</t>
   </si>
   <si>
-    <t>2;3</t>
+    <t>meal:20:0:free/drink:1:1:cash</t>
+  </si>
+  <si>
+    <t>meal:20:0:free/cotton-candy:1:1:cash;meal:10:5:cash/drink:1:1:e-transfer</t>
+  </si>
+  <si>
+    <t>Y23-price</t>
   </si>
 </sst>
 </file>
@@ -678,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH3"/>
+  <dimension ref="A1:BI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AS1" sqref="AS1:AS1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -700,10 +706,11 @@
     <col min="44" max="44" width="24.83203125" customWidth="1"/>
     <col min="46" max="46" width="27.6640625" customWidth="1"/>
     <col min="47" max="47" width="47" customWidth="1"/>
-    <col min="58" max="58" width="16" customWidth="1"/>
+    <col min="48" max="48" width="11.1640625" customWidth="1"/>
+    <col min="59" max="59" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -846,46 +853,49 @@
         <v>46</v>
       </c>
       <c r="AV1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>90</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -946,26 +956,29 @@
       <c r="AU2" t="s">
         <v>88</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AV2">
+        <v>20</v>
+      </c>
+      <c r="AW2" t="s">
         <v>87</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>1</v>
       </c>
-      <c r="AX2">
-        <v>5</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="BD2">
-        <v>0</v>
-      </c>
-      <c r="BH2">
+      <c r="AY2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1059,43 +1072,46 @@
       <c r="AU3" t="s">
         <v>79</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AV3">
+        <v>10</v>
+      </c>
+      <c r="AW3" t="s">
         <v>61</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>1</v>
       </c>
-      <c r="AX3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY3">
+      <c r="AY3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ3">
         <v>1</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BA3" t="s">
         <v>62</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BB3" t="s">
         <v>63</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BC3" t="s">
         <v>64</v>
       </c>
-      <c r="BC3">
-        <v>0</v>
-      </c>
       <c r="BD3">
+        <v>0</v>
+      </c>
+      <c r="BE3">
         <v>1</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BF3" t="s">
         <v>62</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BG3" t="s">
         <v>65</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BH3" t="s">
         <v>64</v>
       </c>
-      <c r="BH3">
+      <c r="BI3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feature: UI improvement (#90)
</commit_message>
<xml_diff>
--- a/__fixtures__/simple.xlsx
+++ b/__fixtures__/simple.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3155266-58A5-A14C-B433-F7C59CCDC0F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92907122-837B-CB4C-A6DD-11192E975B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="94">
   <si>
     <t>Address</t>
   </si>
@@ -290,7 +290,13 @@
     <t>Y23-ticket</t>
   </si>
   <si>
-    <t>2;3</t>
+    <t>meal:20:0:free/drink:1:1:cash</t>
+  </si>
+  <si>
+    <t>meal:20:0:free/cotton-candy:1:1:cash;meal:10:5:cash/drink:1:1:e-transfer</t>
+  </si>
+  <si>
+    <t>Y23-price</t>
   </si>
 </sst>
 </file>
@@ -678,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH3"/>
+  <dimension ref="A1:BI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AS1" sqref="AS1:AS1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -700,10 +706,11 @@
     <col min="44" max="44" width="24.83203125" customWidth="1"/>
     <col min="46" max="46" width="27.6640625" customWidth="1"/>
     <col min="47" max="47" width="47" customWidth="1"/>
-    <col min="58" max="58" width="16" customWidth="1"/>
+    <col min="48" max="48" width="11.1640625" customWidth="1"/>
+    <col min="59" max="59" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -846,46 +853,49 @@
         <v>46</v>
       </c>
       <c r="AV1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>90</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>50</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>51</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>52</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>53</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>54</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>56</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>57</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -946,26 +956,29 @@
       <c r="AU2" t="s">
         <v>88</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AV2">
+        <v>20</v>
+      </c>
+      <c r="AW2" t="s">
         <v>87</v>
       </c>
-      <c r="AW2">
+      <c r="AX2">
         <v>1</v>
       </c>
-      <c r="AX2">
-        <v>5</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="BD2">
-        <v>0</v>
-      </c>
-      <c r="BH2">
+      <c r="AY2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BE2">
+        <v>0</v>
+      </c>
+      <c r="BI2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -1059,43 +1072,46 @@
       <c r="AU3" t="s">
         <v>79</v>
       </c>
-      <c r="AV3" t="s">
+      <c r="AV3">
+        <v>10</v>
+      </c>
+      <c r="AW3" t="s">
         <v>61</v>
       </c>
-      <c r="AW3">
+      <c r="AX3">
         <v>1</v>
       </c>
-      <c r="AX3" t="s">
-        <v>91</v>
-      </c>
-      <c r="AY3">
+      <c r="AY3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AZ3">
         <v>1</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BA3" t="s">
         <v>62</v>
       </c>
-      <c r="BA3" t="s">
+      <c r="BB3" t="s">
         <v>63</v>
       </c>
-      <c r="BB3" t="s">
+      <c r="BC3" t="s">
         <v>64</v>
       </c>
-      <c r="BC3">
-        <v>0</v>
-      </c>
       <c r="BD3">
+        <v>0</v>
+      </c>
+      <c r="BE3">
         <v>1</v>
       </c>
-      <c r="BE3" t="s">
+      <c r="BF3" t="s">
         <v>62</v>
       </c>
-      <c r="BF3" t="s">
+      <c r="BG3" t="s">
         <v>65</v>
       </c>
-      <c r="BG3" t="s">
+      <c r="BH3" t="s">
         <v>64</v>
       </c>
-      <c r="BH3">
+      <c r="BI3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: event ticket sale
</commit_message>
<xml_diff>
--- a/__fixtures__/simple.xlsx
+++ b/__fixtures__/simple.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92907122-837B-CB4C-A6DD-11192E975B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D95383-8E17-F742-8FE8-0EB4B80599B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65880" yWindow="-600" windowWidth="33940" windowHeight="26860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCRA membership" sheetId="1" r:id="rId1"/>
@@ -293,10 +293,10 @@
     <t>meal:20:0:free/drink:1:1:cash</t>
   </si>
   <si>
-    <t>meal:20:0:free/cotton-candy:1:1:cash;meal:10:5:cash/drink:1:1:e-transfer</t>
-  </si>
-  <si>
     <t>Y23-price</t>
+  </si>
+  <si>
+    <t>meal:20:0:free/cotton-candy:1:1:cash;meal:10:5:cash/drink:1:1:e-Transfer</t>
   </si>
 </sst>
 </file>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AV2" sqref="AV2"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AY3" sqref="AY3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -707,6 +707,7 @@
     <col min="46" max="46" width="27.6640625" customWidth="1"/>
     <col min="47" max="47" width="47" customWidth="1"/>
     <col min="48" max="48" width="11.1640625" customWidth="1"/>
+    <col min="51" max="51" width="72.5" customWidth="1"/>
     <col min="59" max="59" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -853,7 +854,7 @@
         <v>46</v>
       </c>
       <c r="AV1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AW1" t="s">
         <v>47</v>
@@ -1082,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="AY3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AZ3">
         <v>1</v>

</xml_diff>

<commit_message>
feature: event ticket sale on dashboard (#92)
</commit_message>
<xml_diff>
--- a/__fixtures__/simple.xlsx
+++ b/__fixtures__/simple.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92907122-837B-CB4C-A6DD-11192E975B83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D95383-8E17-F742-8FE8-0EB4B80599B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="500" windowWidth="49520" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="65880" yWindow="-600" windowWidth="33940" windowHeight="26860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LCRA membership" sheetId="1" r:id="rId1"/>
@@ -293,10 +293,10 @@
     <t>meal:20:0:free/drink:1:1:cash</t>
   </si>
   <si>
-    <t>meal:20:0:free/cotton-candy:1:1:cash;meal:10:5:cash/drink:1:1:e-transfer</t>
-  </si>
-  <si>
     <t>Y23-price</t>
+  </si>
+  <si>
+    <t>meal:20:0:free/cotton-candy:1:1:cash;meal:10:5:cash/drink:1:1:e-Transfer</t>
   </si>
 </sst>
 </file>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK1" workbookViewId="0">
-      <selection activeCell="AV2" sqref="AV2"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="AY3" sqref="AY3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -707,6 +707,7 @@
     <col min="46" max="46" width="27.6640625" customWidth="1"/>
     <col min="47" max="47" width="47" customWidth="1"/>
     <col min="48" max="48" width="11.1640625" customWidth="1"/>
+    <col min="51" max="51" width="72.5" customWidth="1"/>
     <col min="59" max="59" width="16" customWidth="1"/>
   </cols>
   <sheetData>
@@ -853,7 +854,7 @@
         <v>46</v>
       </c>
       <c r="AV1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="AW1" t="s">
         <v>47</v>
@@ -1082,7 +1083,7 @@
         <v>1</v>
       </c>
       <c r="AY3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="AZ3">
         <v>1</v>

</xml_diff>

<commit_message>
feat: import/export to multi-sheet (#157)
</commit_message>
<xml_diff>
--- a/__fixtures__/simple.xlsx
+++ b/__fixtures__/simple.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D95383-8E17-F742-8FE8-0EB4B80599B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D2FD1F-9472-BF42-9EC0-D4AE4C9794A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="65880" yWindow="-600" windowWidth="33940" windowHeight="26860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="LCRA membership" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample Community" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>

</xml_diff>